<commit_message>
Update: set de datos actualizado
</commit_message>
<xml_diff>
--- a/backend/data/candidatos.xlsx
+++ b/backend/data/candidatos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lautaro Roca Vilte\tp-inicial-lcs-ml-rrhh\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lautaro Roca Vilte\tp-inicial-lcs-ml-rrhh\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C4EFEF-7F80-44F1-9836-6700655B8675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF75EA0-9E12-49AC-A17A-FE9155D56E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="180">
   <si>
     <t>nivel_educativo</t>
   </si>
@@ -310,6 +310,264 @@
   </si>
   <si>
     <t>anios_de_experiencia</t>
+  </si>
+  <si>
+    <t>esteban castro</t>
+  </si>
+  <si>
+    <t>Java, JavaScript, SQL</t>
+  </si>
+  <si>
+    <t>Francés, Portugués</t>
+  </si>
+  <si>
+    <t>silvia herrera</t>
+  </si>
+  <si>
+    <t>Python, Excel</t>
+  </si>
+  <si>
+    <t>Inglés</t>
+  </si>
+  <si>
+    <t>rosa ruiz</t>
+  </si>
+  <si>
+    <t>Python, SQL, JavaScript</t>
+  </si>
+  <si>
+    <t>Portugués, Inglés</t>
+  </si>
+  <si>
+    <t>ana romero</t>
+  </si>
+  <si>
+    <t>SQL, Python</t>
+  </si>
+  <si>
+    <t>Francés</t>
+  </si>
+  <si>
+    <t>andrés sánchez</t>
+  </si>
+  <si>
+    <t>Excel, JavaScript, SQL</t>
+  </si>
+  <si>
+    <t>teresa herrera</t>
+  </si>
+  <si>
+    <t>JavaScript, SQL</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>santiago torres</t>
+  </si>
+  <si>
+    <t>JavaScript, Java, Python</t>
+  </si>
+  <si>
+    <t>alicia sánchez</t>
+  </si>
+  <si>
+    <t>Python, SQL, Excel</t>
+  </si>
+  <si>
+    <t>Francés, Inglés</t>
+  </si>
+  <si>
+    <t>SQL, Excel, Java</t>
+  </si>
+  <si>
+    <t>alicia morales</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Portugués, Francés</t>
+  </si>
+  <si>
+    <t>marcos romero</t>
+  </si>
+  <si>
+    <t>rosa torres</t>
+  </si>
+  <si>
+    <t>Inglés, Portugués</t>
+  </si>
+  <si>
+    <t>patricia ramos</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>raquel silva</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>hugo gonzález</t>
+  </si>
+  <si>
+    <t>Java, Python</t>
+  </si>
+  <si>
+    <t>Portugués</t>
+  </si>
+  <si>
+    <t>juan garcía</t>
+  </si>
+  <si>
+    <t>Java, Python, JavaScript, SQL</t>
+  </si>
+  <si>
+    <t>Inglés, Francés</t>
+  </si>
+  <si>
+    <t>teresa lópez</t>
+  </si>
+  <si>
+    <t>santiago muñoz</t>
+  </si>
+  <si>
+    <t>Excel, Java, Python</t>
+  </si>
+  <si>
+    <t>Portugués, Inglés, Francés</t>
+  </si>
+  <si>
+    <t>marcos sánchez</t>
+  </si>
+  <si>
+    <t>Portugués, Francés, Inglés</t>
+  </si>
+  <si>
+    <t>miguel fernández</t>
+  </si>
+  <si>
+    <t>Excel, SQL, JavaScript</t>
+  </si>
+  <si>
+    <t>josé díaz</t>
+  </si>
+  <si>
+    <t>SQL, JavaScript, Python, Java</t>
+  </si>
+  <si>
+    <t>carmen romero</t>
+  </si>
+  <si>
+    <t>JavaScript, SQL, Excel, Java</t>
+  </si>
+  <si>
+    <t>sandra silva</t>
+  </si>
+  <si>
+    <t>JavaScript, Python, Excel</t>
+  </si>
+  <si>
+    <t>Inglés, Francés, Portugués</t>
+  </si>
+  <si>
+    <t>ana herrera</t>
+  </si>
+  <si>
+    <t>JavaScript, SQL, Excel</t>
+  </si>
+  <si>
+    <t>marta pérez</t>
+  </si>
+  <si>
+    <t>Python, SQL</t>
+  </si>
+  <si>
+    <t>sebastián díaz</t>
+  </si>
+  <si>
+    <t>ana castro</t>
+  </si>
+  <si>
+    <t>ana ruiz</t>
+  </si>
+  <si>
+    <t>JavaScript, Excel</t>
+  </si>
+  <si>
+    <t>federico muñoz</t>
+  </si>
+  <si>
+    <t>susana silva</t>
+  </si>
+  <si>
+    <t>SQL, JavaScript</t>
+  </si>
+  <si>
+    <t>maría herrera</t>
+  </si>
+  <si>
+    <t>JavaScript, Java, SQL</t>
+  </si>
+  <si>
+    <t>Inglés, Portugués, Francés</t>
+  </si>
+  <si>
+    <t>maría muñoz</t>
+  </si>
+  <si>
+    <t>alberto gonzález</t>
+  </si>
+  <si>
+    <t>carolina ramos</t>
+  </si>
+  <si>
+    <t>Python, Excel, JavaScript, Java</t>
+  </si>
+  <si>
+    <t>Python, Sql, Java</t>
+  </si>
+  <si>
+    <t>lourdes jiménez</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>francisco gonzález</t>
+  </si>
+  <si>
+    <t>Excel, SQL</t>
+  </si>
+  <si>
+    <t>verónica romero</t>
+  </si>
+  <si>
+    <t>carolina jiménez</t>
+  </si>
+  <si>
+    <t>teresa sánchez</t>
+  </si>
+  <si>
+    <t>carolina ruiz</t>
+  </si>
+  <si>
+    <t>andrés torres</t>
+  </si>
+  <si>
+    <t>martín díaz</t>
+  </si>
+  <si>
+    <t>SQL, Java</t>
+  </si>
+  <si>
+    <t>carolina fernández</t>
+  </si>
+  <si>
+    <t>santiago romero</t>
   </si>
 </sst>
 </file>
@@ -360,16 +618,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,28 +957,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="1" customWidth="1"/>
-    <col min="7" max="8" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="1" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -714,10 +989,10 @@
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -728,10 +1003,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="1">
@@ -740,10 +1015,10 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G2" s="1">
@@ -754,33 +1029,33 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>47</v>
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
+      <c r="E3" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G3" s="1">
-        <v>3500000</v>
+        <v>2100000</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="1">
@@ -789,10 +1064,10 @@
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="8" t="s">
         <v>89</v>
       </c>
       <c r="G4" s="1">
@@ -803,10 +1078,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="1">
@@ -815,10 +1090,10 @@
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="8" t="s">
         <v>90</v>
       </c>
       <c r="G5" s="1">
@@ -829,36 +1104,36 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>58</v>
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>89</v>
+      <c r="E6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="G6" s="1">
-        <v>3150000</v>
+        <v>2200000</v>
       </c>
       <c r="H6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="1">
@@ -867,24 +1142,24 @@
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G7" s="1">
         <v>3600000</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="1">
@@ -893,10 +1168,10 @@
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G8" s="1">
@@ -907,33 +1182,36 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>39</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>72</v>
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="C9" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>17</v>
+      <c r="E9" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="G9" s="1">
-        <v>3100000</v>
+        <v>2700000</v>
       </c>
       <c r="H9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="1">
@@ -942,7 +1220,7 @@
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="8" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="1">
@@ -953,10 +1231,10 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C11" s="1">
@@ -965,7 +1243,7 @@
       <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="1">
@@ -976,10 +1254,10 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="1">
@@ -988,10 +1266,10 @@
       <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G12" s="1">
@@ -1002,112 +1280,109 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>47</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>80</v>
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="C13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>89</v>
+      <c r="E13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="G13" s="1">
-        <v>3000000</v>
+        <v>2850000</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>45</v>
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="C14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>88</v>
+      <c r="E14" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="G14" s="1">
-        <v>2850000</v>
+        <v>2500000</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>8</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>41</v>
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C15" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>87</v>
+      <c r="E15" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="G15" s="1">
-        <v>2700000</v>
+        <v>3500000</v>
       </c>
       <c r="H15" s="1">
-        <v>1</v>
-      </c>
-      <c r="J15" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="1">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="8" t="s">
         <v>92</v>
       </c>
       <c r="G16" s="1">
-        <v>2800000</v>
+        <v>4100000</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="1">
@@ -1116,10 +1391,10 @@
       <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G17" s="1">
@@ -1130,10 +1405,10 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="1">
@@ -1142,10 +1417,10 @@
       <c r="D18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G18" s="1">
@@ -1156,10 +1431,10 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="10">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="1">
@@ -1168,7 +1443,7 @@
       <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G19" s="1">
@@ -1179,10 +1454,10 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="10">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C20" s="1">
@@ -1191,7 +1466,7 @@
       <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="1">
@@ -1202,10 +1477,10 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="10">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="7" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="1">
@@ -1214,10 +1489,10 @@
       <c r="D21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G21" s="1">
@@ -1228,10 +1503,10 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="10">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="1">
@@ -1240,10 +1515,10 @@
       <c r="D22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G22" s="1">
@@ -1254,10 +1529,10 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="10">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C23" s="1">
@@ -1266,10 +1541,10 @@
       <c r="D23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G23" s="1">
@@ -1280,10 +1555,10 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="10">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C24" s="1">
@@ -1292,10 +1567,10 @@
       <c r="D24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G24" s="1">
@@ -1306,10 +1581,10 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="10">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C25" s="1">
@@ -1318,7 +1593,7 @@
       <c r="D25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="1">
@@ -1329,11 +1604,11 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>45</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>78</v>
+      <c r="A26" s="10">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
@@ -1341,24 +1616,24 @@
       <c r="D26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>88</v>
+      <c r="E26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="G26" s="1">
-        <v>2700000</v>
+        <v>3150000</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="10">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C27" s="1">
@@ -1367,10 +1642,10 @@
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="8" t="s">
         <v>89</v>
       </c>
       <c r="G27" s="1">
@@ -1381,10 +1656,10 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C28" s="1">
@@ -1393,10 +1668,10 @@
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G28" s="1">
@@ -1407,10 +1682,10 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="10">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="1">
@@ -1419,10 +1694,10 @@
       <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="8" t="s">
         <v>89</v>
       </c>
       <c r="G29" s="1">
@@ -1433,10 +1708,10 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="10">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C30" s="1">
@@ -1445,7 +1720,7 @@
       <c r="D30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G30" s="1">
@@ -1456,10 +1731,10 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="10">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="1">
@@ -1468,7 +1743,7 @@
       <c r="D31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="8" t="s">
         <v>27</v>
       </c>
       <c r="G31" s="1">
@@ -1479,10 +1754,10 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32" s="10">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="1">
@@ -1491,7 +1766,7 @@
       <c r="D32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="8" t="s">
         <v>28</v>
       </c>
       <c r="G32" s="1">
@@ -1502,10 +1777,10 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33" s="10">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C33" s="1">
@@ -1514,10 +1789,10 @@
       <c r="D33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G33" s="1">
@@ -1528,10 +1803,10 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="10">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C34" s="1">
@@ -1540,10 +1815,10 @@
       <c r="D34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="8" t="s">
         <v>90</v>
       </c>
       <c r="G34" s="1">
@@ -1554,11 +1829,11 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>13</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>46</v>
+      <c r="A35" s="10">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
@@ -1566,21 +1841,24 @@
       <c r="D35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>10</v>
+      <c r="E35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="G35" s="1">
-        <v>2500000</v>
+        <v>2450000</v>
       </c>
       <c r="H35" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36" s="10">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C36" s="1">
@@ -1589,10 +1867,10 @@
       <c r="D36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="8" t="s">
         <v>89</v>
       </c>
       <c r="G36" s="1">
@@ -1603,10 +1881,10 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37" s="10">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="7" t="s">
         <v>69</v>
       </c>
       <c r="C37" s="1">
@@ -1615,10 +1893,10 @@
       <c r="D37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="8" t="s">
         <v>89</v>
       </c>
       <c r="G37" s="1">
@@ -1629,10 +1907,10 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="A38" s="10">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C38" s="1">
@@ -1641,7 +1919,7 @@
       <c r="D38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="8" t="s">
         <v>31</v>
       </c>
       <c r="G38" s="1">
@@ -1652,10 +1930,10 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="A39" s="10">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C39" s="1">
@@ -1664,7 +1942,7 @@
       <c r="D39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="8" t="s">
         <v>30</v>
       </c>
       <c r="G39" s="1">
@@ -1675,36 +1953,33 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>34</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>67</v>
+      <c r="A40" s="10">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="C40" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>91</v>
+      <c r="E40" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G40" s="1">
-        <v>2450000</v>
+        <v>3100000</v>
       </c>
       <c r="H40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41" s="10">
         <v>40</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C41" s="1">
@@ -1713,7 +1988,7 @@
       <c r="D41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G41" s="1">
@@ -1724,10 +1999,10 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="A42" s="10">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="7" t="s">
         <v>74</v>
       </c>
       <c r="C42" s="1">
@@ -1736,10 +2011,10 @@
       <c r="D42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" s="8" t="s">
         <v>90</v>
       </c>
       <c r="G42" s="1">
@@ -1750,10 +2025,10 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="A43" s="10">
         <v>42</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C43" s="1">
@@ -1762,10 +2037,10 @@
       <c r="D43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="8" t="s">
         <v>90</v>
       </c>
       <c r="G43" s="1">
@@ -1776,10 +2051,10 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="A44" s="10">
         <v>43</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C44" s="1">
@@ -1788,10 +2063,10 @@
       <c r="D44" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G44" s="1">
@@ -1802,59 +2077,62 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>5</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>38</v>
+      <c r="A45" s="10">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="C45" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="E45" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G45" s="1">
-        <v>2200000</v>
+        <v>1600000</v>
       </c>
       <c r="H45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="A46" s="10">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="1">
         <v>2</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="1">
-        <v>7</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="F46" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="G46" s="1">
-        <v>2100000</v>
+        <v>2700000</v>
       </c>
       <c r="H46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+      <c r="A47" s="10">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="7" t="s">
         <v>79</v>
       </c>
       <c r="C47" s="1">
@@ -1863,10 +2141,10 @@
       <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G47" s="1">
@@ -1877,11 +2155,11 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>44</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>77</v>
+      <c r="A48" s="10">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="C48" s="1">
         <v>0</v>
@@ -1889,24 +2167,24 @@
       <c r="D48" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>88</v>
+      <c r="E48" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="G48" s="1">
-        <v>1600000</v>
+        <v>3000000</v>
       </c>
       <c r="H48" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="7" t="s">
         <v>81</v>
       </c>
       <c r="C49" s="1">
@@ -1915,7 +2193,7 @@
       <c r="D49" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="8" t="s">
         <v>14</v>
       </c>
       <c r="G49" s="1">
@@ -1925,11 +2203,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
         <v>49</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="7" t="s">
         <v>82</v>
       </c>
       <c r="C50" s="1">
@@ -1938,10 +2216,10 @@
       <c r="D50" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" s="8" t="s">
         <v>89</v>
       </c>
       <c r="G50" s="1">
@@ -1951,11 +2229,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="10">
         <v>50</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="7" t="s">
         <v>83</v>
       </c>
       <c r="C51" s="1">
@@ -1964,7 +2242,7 @@
       <c r="D51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G51" s="1">
@@ -1974,10 +2252,1397 @@
         <v>0</v>
       </c>
     </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="11">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="6">
+        <v>2</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G52" s="6">
+        <v>2400000</v>
+      </c>
+      <c r="H52" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="10">
+        <v>52</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="1">
+        <v>3</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G53" s="1">
+        <v>2500000</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="10">
+        <v>53</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="1">
+        <v>13</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G54" s="1">
+        <v>3800000</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="11">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="6">
+        <v>11</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G55" s="6">
+        <v>3600000</v>
+      </c>
+      <c r="H55" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="10">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F56" s="9"/>
+      <c r="G56" s="6">
+        <v>2400000</v>
+      </c>
+      <c r="H56" s="6">
+        <v>0</v>
+      </c>
+      <c r="I56"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="10">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G57" s="6">
+        <v>4000000</v>
+      </c>
+      <c r="H57" s="6">
+        <v>1</v>
+      </c>
+      <c r="I57"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="11">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G58" s="6">
+        <v>2700000</v>
+      </c>
+      <c r="H58" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="10">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G59" s="6">
+        <v>2800000</v>
+      </c>
+      <c r="H59" s="6">
+        <v>1</v>
+      </c>
+      <c r="I59"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="10">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60">
+        <v>13</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G60" s="6">
+        <v>3800000</v>
+      </c>
+      <c r="H60" s="6">
+        <v>1</v>
+      </c>
+      <c r="I60"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="11">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61">
+        <v>10</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G61" s="6">
+        <v>3500000</v>
+      </c>
+      <c r="H61" s="6">
+        <v>0</v>
+      </c>
+      <c r="I61"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="11">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62">
+        <v>9</v>
+      </c>
+      <c r="D62" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G62" s="6">
+        <v>2900000</v>
+      </c>
+      <c r="H62" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="10">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G63" s="6">
+        <v>2100000</v>
+      </c>
+      <c r="H63" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="11">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F64" s="9"/>
+      <c r="G64" s="6">
+        <v>2400000</v>
+      </c>
+      <c r="H64" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="11">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G65" s="6">
+        <v>2000000</v>
+      </c>
+      <c r="H65" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="10">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>125</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F66" s="9"/>
+      <c r="G66" s="6">
+        <v>2300000</v>
+      </c>
+      <c r="H66" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="11">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G67" s="6">
+        <v>2200000</v>
+      </c>
+      <c r="H67" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="11">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68">
+        <v>14</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G68" s="6">
+        <v>3900000</v>
+      </c>
+      <c r="H68" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="11">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>123</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G69" s="6">
+        <v>2000000</v>
+      </c>
+      <c r="H69" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="10">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>125</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F70" s="9"/>
+      <c r="G70" s="6">
+        <v>2300000</v>
+      </c>
+      <c r="H70" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="11">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>7</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G71" s="6">
+        <v>9999999</v>
+      </c>
+      <c r="H71" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="10">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>133</v>
+      </c>
+      <c r="C72">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G72" s="6">
+        <v>3300000</v>
+      </c>
+      <c r="H72" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="11">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G73" s="6">
+        <v>2900000</v>
+      </c>
+      <c r="H73" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="10">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>137</v>
+      </c>
+      <c r="C74">
+        <v>5</v>
+      </c>
+      <c r="D74" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G74" s="6">
+        <v>3000000</v>
+      </c>
+      <c r="H74" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="11">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>139</v>
+      </c>
+      <c r="C75">
+        <v>7</v>
+      </c>
+      <c r="D75" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F75" s="9"/>
+      <c r="G75" s="6">
+        <v>7500000</v>
+      </c>
+      <c r="H75" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="10">
+        <v>75</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C76" s="1">
+        <v>14</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="G76" s="1">
+        <v>3900000</v>
+      </c>
+      <c r="H76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="11">
+        <v>76</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C77" s="1">
+        <v>13</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G77" s="1">
+        <v>3500000</v>
+      </c>
+      <c r="H77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="10">
+        <v>77</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C78" s="1">
+        <v>10</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="G78" s="1">
+        <v>3500000</v>
+      </c>
+      <c r="H78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="11">
+        <v>78</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C79" s="1">
+        <v>13</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G79" s="1">
+        <v>3800000</v>
+      </c>
+      <c r="H79" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="10">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>150</v>
+      </c>
+      <c r="C80">
+        <v>7</v>
+      </c>
+      <c r="D80" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G80" s="6">
+        <v>3200000</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="11">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81">
+        <v>15</v>
+      </c>
+      <c r="D81" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F81" s="9"/>
+      <c r="G81" s="6">
+        <v>3700000</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="10">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>153</v>
+      </c>
+      <c r="C82">
+        <v>3</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G82" s="6">
+        <v>2800000</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="11">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>154</v>
+      </c>
+      <c r="C83">
+        <v>5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G83" s="6">
+        <v>3000000</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="10">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>156</v>
+      </c>
+      <c r="C84">
+        <v>10</v>
+      </c>
+      <c r="D84" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G84" s="6">
+        <v>3200000</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="11">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>157</v>
+      </c>
+      <c r="C85">
+        <v>3</v>
+      </c>
+      <c r="D85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G85" s="6">
+        <v>2500000</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="10">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>159</v>
+      </c>
+      <c r="C86">
+        <v>7</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G86" s="6">
+        <v>3200000</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="11">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>162</v>
+      </c>
+      <c r="C87">
+        <v>7</v>
+      </c>
+      <c r="D87" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F87" s="9"/>
+      <c r="G87" s="6">
+        <v>2700000</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="10">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>111</v>
+      </c>
+      <c r="C88">
+        <v>5</v>
+      </c>
+      <c r="D88" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G88" s="6">
+        <v>2700000</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="11">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>163</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G89" s="6">
+        <v>2300000</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="10">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>164</v>
+      </c>
+      <c r="C90">
+        <v>11</v>
+      </c>
+      <c r="D90" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G90" s="6">
+        <v>7500000</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="11">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>167</v>
+      </c>
+      <c r="C91">
+        <v>6</v>
+      </c>
+      <c r="D91" t="s">
+        <v>7</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G91" s="6">
+        <v>2600000</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="10">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>169</v>
+      </c>
+      <c r="C92">
+        <v>10</v>
+      </c>
+      <c r="D92" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G92" s="6">
+        <v>3200000</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="11">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>171</v>
+      </c>
+      <c r="C93">
+        <v>6</v>
+      </c>
+      <c r="D93" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G93" s="6">
+        <v>2600000</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="10">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>172</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F94" s="9"/>
+      <c r="G94" s="6">
+        <v>2000000</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="11">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>173</v>
+      </c>
+      <c r="C95">
+        <v>8</v>
+      </c>
+      <c r="D95" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G95" s="6">
+        <v>2800000</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="10">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>174</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F96" s="9"/>
+      <c r="G96" s="6">
+        <v>2200000</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="11">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>175</v>
+      </c>
+      <c r="C97">
+        <v>4</v>
+      </c>
+      <c r="D97" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G97" s="6">
+        <v>2900000</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="10">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>176</v>
+      </c>
+      <c r="C98">
+        <v>9</v>
+      </c>
+      <c r="D98" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G98" s="6">
+        <v>2900000</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="11">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>178</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F99" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G99" s="6">
+        <v>2300000</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="11">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>179</v>
+      </c>
+      <c r="C100">
+        <v>3</v>
+      </c>
+      <c r="D100" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G100" s="6">
+        <v>2800000</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="10">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>49</v>
+      </c>
+      <c r="C101">
+        <v>8</v>
+      </c>
+      <c r="D101" t="s">
+        <v>7</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G101" s="6">
+        <v>2800000</v>
+      </c>
+      <c r="H101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="11"/>
+      <c r="B102"/>
+      <c r="C102"/>
+      <c r="D102"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="6"/>
+      <c r="H102"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B103"/>
+      <c r="C103"/>
+      <c r="D103"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="6"/>
+      <c r="H103"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="11"/>
+      <c r="B104"/>
+      <c r="C104"/>
+      <c r="D104"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="6"/>
+      <c r="H104"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B105"/>
+      <c r="C105"/>
+      <c r="D105"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="6"/>
+      <c r="H105"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B106"/>
+      <c r="C106"/>
+      <c r="D106"/>
+      <c r="E106"/>
+      <c r="F106"/>
+      <c r="G106" s="6"/>
+      <c r="H106"/>
+      <c r="I106"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="11"/>
+      <c r="B107"/>
+      <c r="C107"/>
+      <c r="D107"/>
+      <c r="E107"/>
+      <c r="F107"/>
+      <c r="G107" s="6"/>
+      <c r="H107"/>
+      <c r="I107"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B108"/>
+      <c r="C108"/>
+      <c r="D108"/>
+      <c r="E108"/>
+      <c r="F108"/>
+      <c r="G108" s="6"/>
+      <c r="H108"/>
+      <c r="I108"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B109"/>
+      <c r="C109"/>
+      <c r="D109"/>
+      <c r="E109"/>
+      <c r="F109"/>
+      <c r="G109" s="6"/>
+      <c r="H109"/>
+      <c r="I109"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="11"/>
+      <c r="B110"/>
+      <c r="C110"/>
+      <c r="D110"/>
+      <c r="E110"/>
+      <c r="F110"/>
+      <c r="G110" s="6"/>
+      <c r="H110"/>
+      <c r="I110"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B111"/>
+      <c r="C111"/>
+      <c r="D111"/>
+      <c r="E111"/>
+      <c r="F111"/>
+      <c r="G111" s="6"/>
+      <c r="H111"/>
+      <c r="I111"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H51" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H48">
-      <sortCondition descending="1" ref="G1:G51"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H51">
+      <sortCondition ref="A1:A51"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>